<commit_message>
Update Progetto Aerodinamico Gestione.xlsx
</commit_message>
<xml_diff>
--- a/Progetto Aerodinamico Gestione.xlsx
+++ b/Progetto Aerodinamico Gestione.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silvi\OneDrive\Documenti\GitHub\progettoAerodinamico\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/silviadanesi/Documents/GitHub/progettoAerodinamico/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F5457D-0C77-48CE-9F44-A9850CAA89E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7292BE70-B0B2-3141-AC1B-FEF4A30894C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{4C7CE075-C1D8-5A41-A05E-4A1762B69073}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" activeTab="2" xr2:uid="{4C7CE075-C1D8-5A41-A05E-4A1762B69073}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Progetto Aerodinamico</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t>Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il mio litigio con ogni tipo di software continua. Sto provando a stimare il campo di moto su python, per poi calcolare i carichi </t>
+  </si>
+  <si>
+    <t>Preghiere</t>
   </si>
 </sst>
 </file>
@@ -568,40 +574,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -625,13 +604,40 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -974,49 +980,49 @@
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.796875" style="1"/>
-    <col min="2" max="2" width="19.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" style="1" customWidth="1"/>
     <col min="4" max="4" width="2" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.796875" style="1"/>
+    <col min="5" max="5" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="27" t="s">
+    <row r="1" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="29"/>
-    </row>
-    <row r="3" spans="2:11" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="32" t="s">
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="20"/>
+    </row>
+    <row r="3" spans="2:11" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="31"/>
-    </row>
-    <row r="4" spans="2:11" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="B4" s="32"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="22"/>
+    </row>
+    <row r="4" spans="2:11" ht="85" x14ac:dyDescent="0.2">
+      <c r="B4" s="23"/>
       <c r="C4" s="6" t="s">
         <v>2</v>
       </c>
@@ -1035,8 +1041,8 @@
       <c r="J4" s="6"/>
       <c r="K4" s="12"/>
     </row>
-    <row r="5" spans="2:11" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="32"/>
+    <row r="5" spans="2:11" ht="102" x14ac:dyDescent="0.2">
+      <c r="B5" s="23"/>
       <c r="C5" s="6" t="s">
         <v>7</v>
       </c>
@@ -1049,8 +1055,8 @@
       <c r="J5" s="6"/>
       <c r="K5" s="12"/>
     </row>
-    <row r="6" spans="2:11" ht="109.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="33"/>
+    <row r="6" spans="2:11" ht="120" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="24"/>
       <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1063,9 +1069,9 @@
       <c r="J6" s="2"/>
       <c r="K6" s="3"/>
     </row>
-    <row r="8" spans="2:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="21" t="s">
+    <row r="8" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="31" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="9" t="s">
@@ -1076,8 +1082,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="22"/>
+    <row r="10" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="32"/>
       <c r="C10" s="8">
         <v>70</v>
       </c>
@@ -1087,8 +1093,8 @@
         <v>394797.73756906076</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="22"/>
+    <row r="11" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="32"/>
       <c r="C11" s="7" t="s">
         <v>12</v>
       </c>
@@ -1097,8 +1103,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="22"/>
+    <row r="12" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="32"/>
       <c r="C12" s="13">
         <f>C10*0.277778</f>
         <v>19.444460000000003</v>
@@ -1108,120 +1114,122 @@
         <v>400000</v>
       </c>
     </row>
-    <row r="13" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="22"/>
-      <c r="C13" s="15" t="s">
+    <row r="13" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="32"/>
+      <c r="C13" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="17"/>
-    </row>
-    <row r="14" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="22"/>
-      <c r="C14" s="24" t="s">
+      <c r="D13" s="26"/>
+      <c r="E13" s="27"/>
+    </row>
+    <row r="14" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="32"/>
+      <c r="C14" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="26"/>
-    </row>
-    <row r="15" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="22"/>
-      <c r="C15" s="15" t="s">
+      <c r="D14" s="35"/>
+      <c r="E14" s="36"/>
+    </row>
+    <row r="15" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="32"/>
+      <c r="C15" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="17"/>
-    </row>
-    <row r="16" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="22"/>
-      <c r="C16" s="24" t="s">
+      <c r="D15" s="26"/>
+      <c r="E15" s="27"/>
+    </row>
+    <row r="16" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="32"/>
+      <c r="C16" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="25"/>
-      <c r="E16" s="26"/>
-    </row>
-    <row r="17" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="22"/>
-      <c r="C17" s="15" t="s">
+      <c r="D16" s="35"/>
+      <c r="E16" s="36"/>
+    </row>
+    <row r="17" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="32"/>
+      <c r="C17" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="17"/>
-    </row>
-    <row r="18" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="22"/>
-      <c r="C18" s="24" t="s">
+      <c r="D17" s="26"/>
+      <c r="E17" s="27"/>
+    </row>
+    <row r="18" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="32"/>
+      <c r="C18" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="25"/>
-      <c r="E18" s="26"/>
-    </row>
-    <row r="19" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="22"/>
-      <c r="C19" s="15" t="s">
+      <c r="D18" s="35"/>
+      <c r="E18" s="36"/>
+    </row>
+    <row r="19" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="32"/>
+      <c r="C19" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="17"/>
-    </row>
-    <row r="20" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="22"/>
-      <c r="C20" s="24" t="s">
+      <c r="D19" s="26"/>
+      <c r="E19" s="27"/>
+    </row>
+    <row r="20" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="32"/>
+      <c r="C20" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="25"/>
-      <c r="E20" s="26"/>
-    </row>
-    <row r="21" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="22"/>
-      <c r="C21" s="15" t="s">
+      <c r="D20" s="35"/>
+      <c r="E20" s="36"/>
+    </row>
+    <row r="21" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="32"/>
+      <c r="C21" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="16"/>
-      <c r="E21" s="17"/>
-    </row>
-    <row r="22" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="22"/>
-      <c r="C22" s="24" t="s">
+      <c r="D21" s="26"/>
+      <c r="E21" s="27"/>
+    </row>
+    <row r="22" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="32"/>
+      <c r="C22" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="25"/>
-      <c r="E22" s="26"/>
-    </row>
-    <row r="23" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="22"/>
-      <c r="C23" s="15" t="s">
+      <c r="D22" s="35"/>
+      <c r="E22" s="36"/>
+    </row>
+    <row r="23" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="32"/>
+      <c r="C23" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="16"/>
-      <c r="E23" s="17"/>
-    </row>
-    <row r="24" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="22"/>
-      <c r="C24" s="24" t="s">
+      <c r="D23" s="26"/>
+      <c r="E23" s="27"/>
+    </row>
+    <row r="24" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="32"/>
+      <c r="C24" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="25"/>
-      <c r="E24" s="26"/>
-    </row>
-    <row r="25" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="22"/>
-      <c r="C25" s="15" t="s">
+      <c r="D24" s="35"/>
+      <c r="E24" s="36"/>
+    </row>
+    <row r="25" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="32"/>
+      <c r="C25" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="16"/>
-      <c r="E25" s="17"/>
-    </row>
-    <row r="26" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="23"/>
-      <c r="C26" s="18" t="s">
+      <c r="D25" s="26"/>
+      <c r="E25" s="27"/>
+    </row>
+    <row r="26" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="33"/>
+      <c r="C26" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="20"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
     <mergeCell ref="B2:K2"/>
     <mergeCell ref="C3:K3"/>
     <mergeCell ref="B3:B6"/>
@@ -1238,8 +1246,6 @@
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C18:E18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1251,7 +1257,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1259,41 +1265,52 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38F1D1E0-6205-B145-9BE0-92EB60575B7D}">
-  <dimension ref="B2:D3"/>
+  <dimension ref="B2:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.19921875" style="1"/>
-    <col min="3" max="3" width="40.09765625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.19921875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.19921875" style="1"/>
+    <col min="1" max="1" width="6.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" style="1"/>
+    <col min="3" max="3" width="40.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="34" t="s">
+    <row r="2" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B2" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="249.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="35">
+    <row r="3" spans="2:4" ht="136" x14ac:dyDescent="0.2">
+      <c r="B3" s="16">
         <v>45771</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="17" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="B4" s="16">
+        <v>45776</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1307,7 +1324,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>